<commit_message>
Fixed bulk import export
</commit_message>
<xml_diff>
--- a/downloads/TUVAT CVS Reports - Data Import Template.xlsx
+++ b/downloads/TUVAT CVS Reports - Data Import Template.xlsx
@@ -1,26 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24334"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\verify-cert-calibration\downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\verify-cert-reports\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8D56867-0D0B-460D-ACEF-C132C375DD80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{848B3413-001E-4626-AC4E-C87FC5C06018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029" forceFullCalc="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>certificate_number</t>
   </si>
@@ -28,15 +42,6 @@
     <t>client_name</t>
   </si>
   <si>
-    <t>equipment_name</t>
-  </si>
-  <si>
-    <t>equipment_brand</t>
-  </si>
-  <si>
-    <t>validity_date</t>
-  </si>
-  <si>
     <t>created_by_email</t>
   </si>
   <si>
@@ -49,39 +54,39 @@
     <t>location</t>
   </si>
   <si>
-    <t>calibrator</t>
-  </si>
-  <si>
-    <t>equipment_id</t>
-  </si>
-  <si>
-    <t>calibration_date</t>
-  </si>
-  <si>
     <t>report_issue_date</t>
   </si>
   <si>
-    <t>calibration_remarks</t>
-  </si>
-  <si>
-    <t>calibration_internal_notes</t>
+    <t>team_members</t>
+  </si>
+  <si>
+    <t>report_prepared_by</t>
+  </si>
+  <si>
+    <t>report_approved_by</t>
+  </si>
+  <si>
+    <t>report_validity_date</t>
+  </si>
+  <si>
+    <t>report_revision</t>
+  </si>
+  <si>
+    <t>report_remarks</t>
+  </si>
+  <si>
+    <t>report_internal_notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -104,9 +109,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -412,77 +416,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1"/>
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.21875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="16.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.77734375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.21875" style="2"/>
+    <col min="1" max="1" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="14.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>